<commit_message>
add contact and tracking in report GI,GR,GT
</commit_message>
<xml_diff>
--- a/netforce_stock/netforce_stock/reports/report_stock_move.xlsx
+++ b/netforce_stock/netforce_stock/reports/report_stock_move.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>{{title}}</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Related To</t>
   </si>
   <si>
+    <t>Contact</t>
+  </si>
+  <si>
     <t>Product Code</t>
   </si>
   <si>
@@ -64,6 +67,9 @@
     <t>Lot/Serial</t>
   </si>
   <si>
+    <t>Tracking</t>
+  </si>
+  <si>
     <t>Loss Qty</t>
   </si>
   <si>
@@ -85,6 +91,9 @@
     <t>{{related}}</t>
   </si>
   <si>
+    <t>{{contact}}</t>
+  </si>
+  <si>
     <t>{{product_code}}</t>
   </si>
   <si>
@@ -113,6 +122,9 @@
   </si>
   <si>
     <t>{{lot}}</t>
+  </si>
+  <si>
+    <t>{{tracking}}</t>
   </si>
   <si>
     <t>{{currency qty_loss}}</t>
@@ -276,8 +288,8 @@
   </sheetPr>
   <dimension ref="1:6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P14" activeCellId="0" sqref="P14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q6" activeCellId="0" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -286,17 +298,17 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.47959183673469"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.1428571428571"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="1" width="20.6989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="51.8163265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.02551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="13" style="1" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="1" width="15.5612244897959"/>
-    <col collapsed="false" hidden="false" max="973" min="18" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="974" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="18.1989795918367"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="51.8163265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.1989795918367"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.02551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.1989795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="14" style="1" width="18.1989795918367"/>
+    <col collapsed="false" hidden="false" max="19" min="17" style="1" width="15.5612244897959"/>
+    <col collapsed="false" hidden="false" max="975" min="20" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="976" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -304,8 +316,6 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="AKL1" s="0"/>
-      <c r="AKM1" s="0"/>
       <c r="AKN1" s="0"/>
       <c r="AKO1" s="0"/>
       <c r="AKP1" s="0"/>
@@ -359,8 +369,6 @@
     <row r="2" s="3" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
       <c r="B2" s="2"/>
-      <c r="AKL2" s="0"/>
-      <c r="AKM2" s="0"/>
       <c r="AKN2" s="0"/>
       <c r="AKO2" s="0"/>
       <c r="AKP2" s="0"/>
@@ -461,8 +469,12 @@
       <c r="Q3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AKL3" s="4"/>
-      <c r="AKM3" s="4"/>
+      <c r="R3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="AKN3" s="4"/>
       <c r="AKO3" s="4"/>
       <c r="AKP3" s="4"/>
@@ -515,12 +527,12 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
-      <c r="F4" s="6"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
@@ -532,60 +544,68 @@
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="K5" s="8" t="s">
         <v>29</v>
       </c>
+      <c r="L5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="N5" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P5" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q5" s="8" t="s">
         <v>33</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -602,6 +622,8 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
missing reference on stock move report
</commit_message>
<xml_diff>
--- a/netforce_stock/netforce_stock/reports/report_stock_move.xlsx
+++ b/netforce_stock/netforce_stock/reports/report_stock_move.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="22" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,127 +13,138 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
-  <si>
-    <t>{{title}}</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Related To</t>
-  </si>
-  <si>
-    <t>Contact</t>
-  </si>
-  <si>
-    <t>Product Code</t>
-  </si>
-  <si>
-    <t>Product Name</t>
-  </si>
-  <si>
-    <t>From Location</t>
-  </si>
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>UoM</t>
-  </si>
-  <si>
-    <t>To Location</t>
-  </si>
-  <si>
-    <t>Secondary Qty</t>
-  </si>
-  <si>
-    <t>From Container</t>
-  </si>
-  <si>
-    <t>To Container</t>
-  </si>
-  <si>
-    <t>Lot/Serial</t>
-  </si>
-  <si>
-    <t>Tracking</t>
-  </si>
-  <si>
-    <t>Loss Qty</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>{{#each lines}}</t>
-  </si>
-  <si>
-    <t>{{_item_no}}</t>
-  </si>
-  <si>
-    <t>{{date}}</t>
-  </si>
-  <si>
-    <t>{{number}}</t>
-  </si>
-  <si>
-    <t>{{related}}</t>
-  </si>
-  <si>
-    <t>{{contact}}</t>
-  </si>
-  <si>
-    <t>{{product_code}}</t>
-  </si>
-  <si>
-    <t>{{product_name}}</t>
-  </si>
-  <si>
-    <t>{{location_from}}</t>
-  </si>
-  <si>
-    <t>{{currency qty}}</t>
-  </si>
-  <si>
-    <t>{{uom}}</t>
-  </si>
-  <si>
-    <t>{{location_to}}</t>
-  </si>
-  <si>
-    <t>{{currency qty2}}</t>
-  </si>
-  <si>
-    <t>{{container_from}}</t>
-  </si>
-  <si>
-    <t>{{container_to}}</t>
-  </si>
-  <si>
-    <t>{{lot}}</t>
-  </si>
-  <si>
-    <t>{{tracking}}</t>
-  </si>
-  <si>
-    <t>{{currency qty_loss}}</t>
-  </si>
-  <si>
-    <t>{{state}}</t>
-  </si>
-  <si>
-    <t>{{/each}}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+  <si>
+    <t xml:space="preserve">{{title}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Related To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary Qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From Container</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To Container</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lot/Serial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tracking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loss Qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ref</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{#each lines}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{_item_no}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{date}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{number}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{related}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{contact}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{product_code}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{product_name}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{location_from}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency qty}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{uom}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{location_to}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency qty2}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{container_from}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{container_to}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{lot}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{tracking}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{currency qty_loss}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{state}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{ref}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{/each}}</t>
   </si>
 </sst>
 </file>
@@ -141,7 +152,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -288,27 +299,26 @@
   </sheetPr>
   <dimension ref="1:6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q6" activeCellId="0" sqref="Q6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T5" activeCellId="0" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.27551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.1428571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="20.6989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="51.8163265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.02551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="16" min="14" style="1" width="18.1989795918367"/>
-    <col collapsed="false" hidden="false" max="19" min="17" style="1" width="15.5612244897959"/>
-    <col collapsed="false" hidden="false" max="975" min="20" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="976" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.20918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="16" min="14" style="1" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="19" min="17" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="975" min="20" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -475,6 +485,9 @@
       <c r="S3" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="T3" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="AKN3" s="4"/>
       <c r="AKO3" s="4"/>
       <c r="AKP3" s="4"/>
@@ -527,7 +540,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -546,66 +559,70 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
+      <c r="T4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -650,7 +667,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.90816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -677,7 +694,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.90816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>